<commit_message>
import to excel successed
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,22 +461,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1234</t>
+          <t>5634</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Honda Goldwing</t>
+          <t>Ninja ZX25R</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>34.000.000</t>
+          <t>45.000.000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2468</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Benelli TRK 502</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>54.000.000</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>40</t>
         </is>
       </c>
     </row>

</xml_diff>